<commit_message>
update for new HCRs
</commit_message>
<xml_diff>
--- a/ibPIL_scenarios.xlsx
+++ b/ibPIL_scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\use\GitHub\FLBEIA_mseIBpil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D343F761-DD70-403F-B049-C90397A2FD4F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677ABA50-B445-4EC6-987A-C0F0E3CF2229}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="30">
   <si>
     <t>SCENARIOS</t>
   </si>
@@ -691,18 +691,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.6640625" customWidth="1"/>
-    <col min="8" max="8" width="55.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.7109375" customWidth="1"/>
+    <col min="8" max="8" width="55.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -713,7 +715,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -730,7 +732,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -745,7 +747,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -762,7 +764,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -776,7 +778,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -790,10 +792,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
@@ -819,7 +821,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>1</v>
       </c>
@@ -846,7 +848,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>2</v>
       </c>
@@ -871,7 +873,7 @@
       </c>
       <c r="H10" s="23"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>3</v>
       </c>
@@ -896,7 +898,7 @@
       </c>
       <c r="H11" s="23"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>4</v>
       </c>
@@ -921,7 +923,7 @@
       </c>
       <c r="H12" s="23"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>5</v>
       </c>
@@ -946,7 +948,7 @@
       </c>
       <c r="H13" s="23"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>6</v>
       </c>
@@ -971,7 +973,7 @@
       </c>
       <c r="H14" s="23"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
@@ -983,7 +985,7 @@
       <c r="G15" s="8"/>
       <c r="H15" s="18"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>7</v>
       </c>
@@ -1010,7 +1012,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>8</v>
       </c>
@@ -1035,7 +1037,7 @@
       </c>
       <c r="H17" s="24"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>9</v>
       </c>
@@ -1060,7 +1062,7 @@
       </c>
       <c r="H18" s="24"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>10</v>
       </c>
@@ -1085,7 +1087,7 @@
       </c>
       <c r="H19" s="24"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="19">
         <v>11</v>
       </c>
@@ -1110,7 +1112,7 @@
       </c>
       <c r="H20" s="24"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
         <v>12</v>
       </c>
@@ -1135,7 +1137,7 @@
       </c>
       <c r="H21" s="24"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9" t="s">
@@ -1147,7 +1149,7 @@
       <c r="G22" s="9"/>
       <c r="H22" s="17"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>13</v>
       </c>
@@ -1174,7 +1176,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>14</v>
       </c>
@@ -1199,7 +1201,7 @@
       </c>
       <c r="H24" s="25"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>15</v>
       </c>
@@ -1224,7 +1226,7 @@
       </c>
       <c r="H25" s="25"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>16</v>
       </c>
@@ -1249,7 +1251,7 @@
       </c>
       <c r="H26" s="25"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>17</v>
       </c>
@@ -1274,7 +1276,7 @@
       </c>
       <c r="H27" s="25"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>18</v>
       </c>
@@ -1299,7 +1301,7 @@
       </c>
       <c r="H28" s="25"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11" t="s">
@@ -1311,7 +1313,7 @@
       <c r="G29" s="11"/>
       <c r="H29" s="16"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>19</v>
       </c>
@@ -1338,7 +1340,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="21">
         <v>20</v>
       </c>
@@ -1363,7 +1365,7 @@
       </c>
       <c r="H31" s="26"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>21</v>
       </c>
@@ -1388,7 +1390,7 @@
       </c>
       <c r="H32" s="26"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="21">
         <v>22</v>
       </c>
@@ -1413,7 +1415,7 @@
       </c>
       <c r="H33" s="26"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>23</v>
       </c>
@@ -1438,7 +1440,7 @@
       </c>
       <c r="H34" s="26"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="21">
         <v>24</v>
       </c>
@@ -1463,7 +1465,7 @@
       </c>
       <c r="H35" s="26"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14" t="s">
@@ -1475,12 +1477,165 @@
       <c r="G36" s="14"/>
       <c r="H36" s="15"/>
     </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="13">
+        <v>25</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" s="14">
+        <v>3</v>
+      </c>
+      <c r="G37" s="14" t="str">
+        <f t="shared" ref="G37:G42" si="4">CONCATENATE("ASS",E37,"_HCR",F37,"_REC",C37,"_INN",B37,"_OER",D37)</f>
+        <v>ASSss3_HCR3_REClow_INNvar_OERnaq</v>
+      </c>
+      <c r="H37" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="21">
+        <v>26</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" s="22">
+        <v>4</v>
+      </c>
+      <c r="G38" s="22" t="str">
+        <f t="shared" si="4"/>
+        <v>ASSss3_HCR4_RECmed_INNvar_OERnaq</v>
+      </c>
+      <c r="H38" s="26"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="13">
+        <v>27</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" s="14">
+        <v>3</v>
+      </c>
+      <c r="G39" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>ASSss3_HCR3_RECmix_INNvar_OERnaq</v>
+      </c>
+      <c r="H39" s="26"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="21">
+        <v>28</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" s="22">
+        <v>4</v>
+      </c>
+      <c r="G40" s="22" t="str">
+        <f t="shared" si="4"/>
+        <v>ASSss3_HCR4_REClow_INNvar_OERnaq</v>
+      </c>
+      <c r="H40" s="26"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="13">
+        <v>29</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F41" s="14">
+        <v>3</v>
+      </c>
+      <c r="G41" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>ASSss3_HCR3_RECmed_INNvar_OERnaq</v>
+      </c>
+      <c r="H41" s="26"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="21">
+        <v>30</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42" s="22">
+        <v>4</v>
+      </c>
+      <c r="G42" s="22" t="str">
+        <f t="shared" si="4"/>
+        <v>ASSss3_HCR4_RECmix_INNvar_OERnaq</v>
+      </c>
+      <c r="H42" s="26"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="H9:H14"/>
     <mergeCell ref="H16:H21"/>
     <mergeCell ref="H23:H28"/>
     <mergeCell ref="H30:H35"/>
+    <mergeCell ref="H37:H42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
new results 100 iters
</commit_message>
<xml_diff>
--- a/ibPIL_scenarios.xlsx
+++ b/ibPIL_scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\use\GitHub\FLBEIA_mseIBpil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677ABA50-B445-4EC6-987A-C0F0E3CF2229}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECED8A65-94BB-4AB9-9D75-04F427FB752E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="30">
   <si>
     <t>SCENARIOS</t>
   </si>
@@ -691,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,8 +1629,161 @@
       </c>
       <c r="H42" s="26"/>
     </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="13">
+        <v>31</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F44" s="14">
+        <v>6</v>
+      </c>
+      <c r="G44" s="14" t="str">
+        <f t="shared" ref="G44:G49" si="5">CONCATENATE("ASS",E44,"_HCR",F44,"_REC",C44,"_INN",B44,"_OER",D44)</f>
+        <v>ASSss3_HCR6_RECmed_INNvar_OERnaq</v>
+      </c>
+      <c r="H44" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="21">
+        <v>32</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F45" s="22">
+        <v>6</v>
+      </c>
+      <c r="G45" s="22" t="str">
+        <f t="shared" si="5"/>
+        <v>ASSss3_HCR6_RECmix_INNvar_OERnaq</v>
+      </c>
+      <c r="H45" s="26"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="13">
+        <v>33</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F46" s="14">
+        <v>5</v>
+      </c>
+      <c r="G46" s="14" t="str">
+        <f t="shared" si="5"/>
+        <v>ASSss3_HCR5_RECmed_INNvar_OERnaq</v>
+      </c>
+      <c r="H46" s="26"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="21">
+        <v>34</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F47" s="22">
+        <v>5</v>
+      </c>
+      <c r="G47" s="22" t="str">
+        <f t="shared" si="5"/>
+        <v>ASSss3_HCR5_RECmix_INNvar_OERnaq</v>
+      </c>
+      <c r="H47" s="26"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="13">
+        <v>35</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F48" s="14">
+        <v>6</v>
+      </c>
+      <c r="G48" s="14" t="str">
+        <f t="shared" si="5"/>
+        <v>ASSss3_HCR6_REClow_INNvar_OERnaq</v>
+      </c>
+      <c r="H48" s="26"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="21">
+        <v>36</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F49" s="22">
+        <v>5</v>
+      </c>
+      <c r="G49" s="22" t="str">
+        <f t="shared" si="5"/>
+        <v>ASSss3_HCR5_REClow_INNvar_OERnaq</v>
+      </c>
+      <c r="H49" s="26"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="H44:H49"/>
     <mergeCell ref="H9:H14"/>
     <mergeCell ref="H16:H21"/>
     <mergeCell ref="H23:H28"/>

</xml_diff>

<commit_message>
HCR 7: no fishing added
</commit_message>
<xml_diff>
--- a/ibPIL_scenarios.xlsx
+++ b/ibPIL_scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\use\GitHub\FLBEIA_mseIBpil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECED8A65-94BB-4AB9-9D75-04F427FB752E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0569E29F-C215-4A5A-840F-307A3E31DE39}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="30">
   <si>
     <t>SCENARIOS</t>
   </si>
@@ -360,6 +360,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -367,9 +370,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -691,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,7 +844,7 @@
         <f t="shared" ref="G9:G14" si="0">CONCATENATE("ASS",E9,"_HCR",F9,"_REC",C9,"_INN",B9,"_OER",D9)</f>
         <v>ASSnone_HCR1_REClow_INNfix_OERnone</v>
       </c>
-      <c r="H9" s="23" t="s">
+      <c r="H9" s="24" t="s">
         <v>22</v>
       </c>
     </row>
@@ -871,7 +871,7 @@
         <f t="shared" si="0"/>
         <v>ASSnone_HCR2_REClow_INNfix_OERnone</v>
       </c>
-      <c r="H10" s="23"/>
+      <c r="H10" s="24"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
@@ -896,7 +896,7 @@
         <f t="shared" si="0"/>
         <v>ASSnone_HCR1_RECmed_INNfix_OERnone</v>
       </c>
-      <c r="H11" s="23"/>
+      <c r="H11" s="24"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
@@ -921,7 +921,7 @@
         <f t="shared" si="0"/>
         <v>ASSnone_HCR2_RECmed_INNfix_OERnone</v>
       </c>
-      <c r="H12" s="23"/>
+      <c r="H12" s="24"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
@@ -946,7 +946,7 @@
         <f t="shared" si="0"/>
         <v>ASSnone_HCR1_RECmix_INNfix_OERnone</v>
       </c>
-      <c r="H13" s="23"/>
+      <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
@@ -971,7 +971,7 @@
         <f t="shared" si="0"/>
         <v>ASSnone_HCR2_RECmix_INNfix_OERnone</v>
       </c>
-      <c r="H14" s="23"/>
+      <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
@@ -1008,7 +1008,7 @@
         <f t="shared" ref="G16:G21" si="1">CONCATENATE("ASS",E16,"_HCR",F16,"_REC",C16,"_INN",B16,"_OER",D16)</f>
         <v>ASSnone_HCR1_REClow_INNvar_OERnone</v>
       </c>
-      <c r="H16" s="24" t="s">
+      <c r="H16" s="25" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1035,7 +1035,7 @@
         <f t="shared" si="1"/>
         <v>ASSnone_HCR2_REClow_INNvar_OERnone</v>
       </c>
-      <c r="H17" s="24"/>
+      <c r="H17" s="25"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
@@ -1060,7 +1060,7 @@
         <f t="shared" si="1"/>
         <v>ASSnone_HCR1_RECmed_INNvar_OERnone</v>
       </c>
-      <c r="H18" s="24"/>
+      <c r="H18" s="25"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
@@ -1085,7 +1085,7 @@
         <f t="shared" si="1"/>
         <v>ASSnone_HCR2_RECmed_INNvar_OERnone</v>
       </c>
-      <c r="H19" s="24"/>
+      <c r="H19" s="25"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="19">
@@ -1110,7 +1110,7 @@
         <f t="shared" si="1"/>
         <v>ASSnone_HCR1_RECmix_INNvar_OERnone</v>
       </c>
-      <c r="H20" s="24"/>
+      <c r="H20" s="25"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
@@ -1135,7 +1135,7 @@
         <f t="shared" si="1"/>
         <v>ASSnone_HCR2_RECmix_INNvar_OERnone</v>
       </c>
-      <c r="H21" s="24"/>
+      <c r="H21" s="25"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
@@ -1172,7 +1172,7 @@
         <f t="shared" ref="G23:G28" si="2">CONCATENATE("ASS",E23,"_HCR",F23,"_REC",C23,"_INN",B23,"_OER",D23)</f>
         <v>ASSemul_HCR1_REClow_INNvar_OERnone</v>
       </c>
-      <c r="H23" s="25" t="s">
+      <c r="H23" s="26" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1199,7 +1199,7 @@
         <f t="shared" si="2"/>
         <v>ASSemul_HCR2_REClow_INNvar_OERnone</v>
       </c>
-      <c r="H24" s="25"/>
+      <c r="H24" s="26"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
@@ -1224,7 +1224,7 @@
         <f t="shared" si="2"/>
         <v>ASSemul_HCR1_RECmed_INNvar_OERnone</v>
       </c>
-      <c r="H25" s="25"/>
+      <c r="H25" s="26"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
@@ -1249,7 +1249,7 @@
         <f t="shared" si="2"/>
         <v>ASSemul_HCR2_RECmed_INNvar_OERnone</v>
       </c>
-      <c r="H26" s="25"/>
+      <c r="H26" s="26"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
@@ -1274,7 +1274,7 @@
         <f t="shared" si="2"/>
         <v>ASSemul_HCR1_RECmix_INNvar_OERnone</v>
       </c>
-      <c r="H27" s="25"/>
+      <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
@@ -1299,7 +1299,7 @@
         <f t="shared" si="2"/>
         <v>ASSemul_HCR2_RECmix_INNvar_OERnone</v>
       </c>
-      <c r="H28" s="25"/>
+      <c r="H28" s="26"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
@@ -1336,7 +1336,7 @@
         <f t="shared" ref="G30:G35" si="3">CONCATENATE("ASS",E30,"_HCR",F30,"_REC",C30,"_INN",B30,"_OER",D30)</f>
         <v>ASSss3_HCR1_REClow_INNvar_OERnaq</v>
       </c>
-      <c r="H30" s="26" t="s">
+      <c r="H30" s="23" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1363,7 +1363,7 @@
         <f t="shared" si="3"/>
         <v>ASSss3_HCR2_RECmed_INNvar_OERnaq</v>
       </c>
-      <c r="H31" s="26"/>
+      <c r="H31" s="23"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
@@ -1388,7 +1388,7 @@
         <f t="shared" si="3"/>
         <v>ASSss3_HCR1_RECmix_INNvar_OERnaq</v>
       </c>
-      <c r="H32" s="26"/>
+      <c r="H32" s="23"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="21">
@@ -1413,7 +1413,7 @@
         <f t="shared" si="3"/>
         <v>ASSss3_HCR2_REClow_INNvar_OERnaq</v>
       </c>
-      <c r="H33" s="26"/>
+      <c r="H33" s="23"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
@@ -1438,7 +1438,7 @@
         <f t="shared" si="3"/>
         <v>ASSss3_HCR1_RECmed_INNvar_OERnaq</v>
       </c>
-      <c r="H34" s="26"/>
+      <c r="H34" s="23"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="21">
@@ -1463,7 +1463,7 @@
         <f t="shared" si="3"/>
         <v>ASSss3_HCR2_RECmix_INNvar_OERnaq</v>
       </c>
-      <c r="H35" s="26"/>
+      <c r="H35" s="23"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
@@ -1500,7 +1500,7 @@
         <f t="shared" ref="G37:G42" si="4">CONCATENATE("ASS",E37,"_HCR",F37,"_REC",C37,"_INN",B37,"_OER",D37)</f>
         <v>ASSss3_HCR3_REClow_INNvar_OERnaq</v>
       </c>
-      <c r="H37" s="26" t="s">
+      <c r="H37" s="23" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1527,7 +1527,7 @@
         <f t="shared" si="4"/>
         <v>ASSss3_HCR4_RECmed_INNvar_OERnaq</v>
       </c>
-      <c r="H38" s="26"/>
+      <c r="H38" s="23"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
@@ -1552,7 +1552,7 @@
         <f t="shared" si="4"/>
         <v>ASSss3_HCR3_RECmix_INNvar_OERnaq</v>
       </c>
-      <c r="H39" s="26"/>
+      <c r="H39" s="23"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="21">
@@ -1577,7 +1577,7 @@
         <f t="shared" si="4"/>
         <v>ASSss3_HCR4_REClow_INNvar_OERnaq</v>
       </c>
-      <c r="H40" s="26"/>
+      <c r="H40" s="23"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="13">
@@ -1602,7 +1602,7 @@
         <f t="shared" si="4"/>
         <v>ASSss3_HCR3_RECmed_INNvar_OERnaq</v>
       </c>
-      <c r="H41" s="26"/>
+      <c r="H41" s="23"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="21">
@@ -1627,7 +1627,7 @@
         <f t="shared" si="4"/>
         <v>ASSss3_HCR4_RECmix_INNvar_OERnaq</v>
       </c>
-      <c r="H42" s="26"/>
+      <c r="H42" s="23"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
@@ -1652,7 +1652,7 @@
         <f t="shared" ref="G44:G49" si="5">CONCATENATE("ASS",E44,"_HCR",F44,"_REC",C44,"_INN",B44,"_OER",D44)</f>
         <v>ASSss3_HCR6_RECmed_INNvar_OERnaq</v>
       </c>
-      <c r="H44" s="26" t="s">
+      <c r="H44" s="23" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1679,7 +1679,7 @@
         <f t="shared" si="5"/>
         <v>ASSss3_HCR6_RECmix_INNvar_OERnaq</v>
       </c>
-      <c r="H45" s="26"/>
+      <c r="H45" s="23"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
@@ -1704,7 +1704,7 @@
         <f t="shared" si="5"/>
         <v>ASSss3_HCR5_RECmed_INNvar_OERnaq</v>
       </c>
-      <c r="H46" s="26"/>
+      <c r="H46" s="23"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="21">
@@ -1729,7 +1729,7 @@
         <f t="shared" si="5"/>
         <v>ASSss3_HCR5_RECmix_INNvar_OERnaq</v>
       </c>
-      <c r="H47" s="26"/>
+      <c r="H47" s="23"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
@@ -1754,7 +1754,7 @@
         <f t="shared" si="5"/>
         <v>ASSss3_HCR6_REClow_INNvar_OERnaq</v>
       </c>
-      <c r="H48" s="26"/>
+      <c r="H48" s="23"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="21">
@@ -1779,7 +1779,79 @@
         <f t="shared" si="5"/>
         <v>ASSss3_HCR5_REClow_INNvar_OERnaq</v>
       </c>
-      <c r="H49" s="26"/>
+      <c r="H49" s="23"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="13">
+        <v>37</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" s="14">
+        <v>7</v>
+      </c>
+      <c r="G51" s="14" t="str">
+        <f t="shared" ref="G51:G53" si="6">CONCATENATE("ASS",E51,"_HCR",F51,"_REC",C51,"_INN",B51,"_OER",D51)</f>
+        <v>ASSnone_HCR7_REClow_INNvar_OERnone</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="21">
+        <v>38</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" s="22">
+        <v>7</v>
+      </c>
+      <c r="G52" s="22" t="str">
+        <f t="shared" si="6"/>
+        <v>ASSnone_HCR7_RECmed_INNvar_OERnone</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="13">
+        <v>39</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" s="14">
+        <v>7</v>
+      </c>
+      <c r="G53" s="14" t="str">
+        <f t="shared" si="6"/>
+        <v>ASSnone_HCR7_RECmix_INNvar_OERnone</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>